<commit_message>
Bug fixes. This version of the model was used in initial manuscript.
</commit_message>
<xml_diff>
--- a/Data/Asthma/Healthcare use/CHARM Healthcare use probs by asthma control.xlsx
+++ b/Data/Asthma/Healthcare use/CHARM Healthcare use probs by asthma control.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smaya\Box\AA_Sigal_Documents\Climate - Health\Wildfire Asthma Microsim\Modeling\Data\Asthma\Healthcare use\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8878AD-8822-4DF8-A0DC-ACEB28409920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E584B02A-B74B-4911-B139-5F121B4A517A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1995" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24240" yWindow="-168" windowWidth="19176" windowHeight="10200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Healthcare use by asthma contro" sheetId="1" r:id="rId1"/>
     <sheet name="Calibration" sheetId="2" r:id="rId2"/>
+    <sheet name="Final results" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="56">
   <si>
     <t>none</t>
   </si>
@@ -233,6 +234,9 @@
   </si>
   <si>
     <t>FIRE - LOADED FIRE ORs (row-wise)</t>
+  </si>
+  <si>
+    <t>Mean proportions</t>
   </si>
 </sst>
 </file>
@@ -1248,7 +1252,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1443,30 +1447,32 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1488,8 +1494,12 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1867,30 +1877,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="J1" s="77" t="s">
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="J1" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="S1" s="76" t="s">
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="S1" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="T1" s="76"/>
-      <c r="U1" s="76"/>
-      <c r="V1" s="76"/>
-      <c r="W1" s="76"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
     </row>
     <row r="2" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B2" s="13" t="s">
@@ -2433,11 +2443,11 @@
         <f>SUM(S3:S10)</f>
         <v>1</v>
       </c>
-      <c r="T11" s="80">
+      <c r="T11" s="76">
         <f>SUM(T3:U10)</f>
         <v>7.1342835938441443E-2</v>
       </c>
-      <c r="U11" s="80"/>
+      <c r="U11" s="76"/>
       <c r="V11" s="6">
         <f>SUM(V3:V10)</f>
         <v>4.9951605660619484E-3</v>
@@ -2453,61 +2463,61 @@
       <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="J12" s="89"/>
-      <c r="K12" s="89"/>
-      <c r="L12" s="89"/>
-      <c r="M12" s="89"/>
-      <c r="N12" s="89"/>
-      <c r="O12" s="89"/>
+      <c r="J12" s="74"/>
+      <c r="K12" s="74"/>
+      <c r="L12" s="74"/>
+      <c r="M12" s="74"/>
+      <c r="N12" s="74"/>
+      <c r="O12" s="74"/>
       <c r="Y12" s="6"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J13" s="90" t="s">
+      <c r="J13" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="K13" s="89" t="s">
-        <v>0</v>
-      </c>
-      <c r="L13" s="89" t="s">
+      <c r="K13" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="L13" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="M13" s="89" t="s">
+      <c r="M13" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="N13" s="89" t="s">
+      <c r="N13" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="O13" s="89" t="s">
+      <c r="O13" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="S13" s="76" t="s">
+      <c r="S13" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="T13" s="76"/>
-      <c r="U13" s="76"/>
-      <c r="V13" s="76"/>
-      <c r="W13" s="76"/>
+      <c r="T13" s="77"/>
+      <c r="U13" s="77"/>
+      <c r="V13" s="77"/>
+      <c r="W13" s="77"/>
     </row>
     <row r="14" spans="1:26" ht="29" x14ac:dyDescent="0.35">
-      <c r="J14" s="89">
-        <v>0</v>
-      </c>
-      <c r="K14" s="89">
+      <c r="J14" s="74">
+        <v>0</v>
+      </c>
+      <c r="K14" s="74">
         <v>1</v>
       </c>
-      <c r="L14" s="89">
-        <v>0</v>
-      </c>
-      <c r="M14" s="89">
-        <v>0</v>
-      </c>
-      <c r="N14" s="89">
-        <v>0</v>
-      </c>
-      <c r="O14" s="89">
+      <c r="L14" s="74">
+        <v>0</v>
+      </c>
+      <c r="M14" s="74">
+        <v>0</v>
+      </c>
+      <c r="N14" s="74">
+        <v>0</v>
+      </c>
+      <c r="O14" s="74">
         <v>0</v>
       </c>
       <c r="S14" s="9" t="s">
@@ -2531,22 +2541,22 @@
       <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="89">
+      <c r="J15" s="74">
         <v>1</v>
       </c>
-      <c r="K15" s="89">
+      <c r="K15" s="74">
         <v>0.91410094600000003</v>
       </c>
-      <c r="L15" s="89">
+      <c r="L15" s="74">
         <v>3.9136651000000001E-2</v>
       </c>
-      <c r="M15" s="89">
+      <c r="M15" s="74">
         <v>4.0466157000000003E-2</v>
       </c>
-      <c r="N15" s="89">
+      <c r="N15" s="74">
         <v>4.3750170000000001E-3</v>
       </c>
-      <c r="O15" s="89">
+      <c r="O15" s="74">
         <v>1.921229E-3</v>
       </c>
       <c r="R15">
@@ -2554,22 +2564,22 @@
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="J16" s="89">
+      <c r="J16" s="74">
         <v>2</v>
       </c>
-      <c r="K16" s="89">
+      <c r="K16" s="74">
         <v>0.88382786199999996</v>
       </c>
-      <c r="L16" s="89">
+      <c r="L16" s="74">
         <v>4.9502009E-2</v>
       </c>
-      <c r="M16" s="89">
+      <c r="M16" s="74">
         <v>5.0963188999999999E-2</v>
       </c>
-      <c r="N16" s="89">
+      <c r="N16" s="74">
         <v>7.3192370000000001E-3</v>
       </c>
-      <c r="O16" s="89">
+      <c r="O16" s="74">
         <v>8.3877020000000004E-3</v>
       </c>
       <c r="R16">
@@ -2599,22 +2609,22 @@
       <c r="A17" t="s">
         <v>11</v>
       </c>
-      <c r="J17" s="89">
+      <c r="J17" s="74">
         <v>3</v>
       </c>
-      <c r="K17" s="89">
+      <c r="K17" s="74">
         <v>0.80730704200000003</v>
       </c>
-      <c r="L17" s="89">
+      <c r="L17" s="74">
         <v>8.0922303000000001E-2</v>
       </c>
-      <c r="M17" s="89">
+      <c r="M17" s="74">
         <v>7.6244352000000001E-2</v>
       </c>
-      <c r="N17" s="89">
+      <c r="N17" s="74">
         <v>1.7045363000000001E-2</v>
       </c>
-      <c r="O17" s="89">
+      <c r="O17" s="74">
         <v>1.8480940000000001E-2</v>
       </c>
       <c r="R17">
@@ -2644,22 +2654,22 @@
       <c r="A18" t="s">
         <v>12</v>
       </c>
-      <c r="J18" s="89">
+      <c r="J18" s="74">
         <v>4</v>
       </c>
-      <c r="K18" s="89">
+      <c r="K18" s="74">
         <v>0.61261256600000003</v>
       </c>
-      <c r="L18" s="89">
+      <c r="L18" s="74">
         <v>0.170907108</v>
       </c>
-      <c r="M18" s="89">
+      <c r="M18" s="74">
         <v>0.136274268</v>
       </c>
-      <c r="N18" s="89">
+      <c r="N18" s="74">
         <v>3.5211289E-2</v>
       </c>
-      <c r="O18" s="89">
+      <c r="O18" s="74">
         <v>4.4994768999999997E-2</v>
       </c>
       <c r="R18">
@@ -2686,22 +2696,22 @@
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="J19" s="89">
+      <c r="J19" s="74">
         <v>5</v>
       </c>
-      <c r="K19" s="89">
+      <c r="K19" s="74">
         <v>0.61261256600000003</v>
       </c>
-      <c r="L19" s="89">
+      <c r="L19" s="74">
         <v>0.170907108</v>
       </c>
-      <c r="M19" s="89">
+      <c r="M19" s="74">
         <v>0.136274268</v>
       </c>
-      <c r="N19" s="89">
+      <c r="N19" s="74">
         <v>3.5211289E-2</v>
       </c>
-      <c r="O19" s="89">
+      <c r="O19" s="74">
         <v>4.4994768999999997E-2</v>
       </c>
       <c r="R19">
@@ -2731,22 +2741,22 @@
       <c r="A20" t="s">
         <v>14</v>
       </c>
-      <c r="J20" s="89">
+      <c r="J20" s="74">
         <v>50</v>
       </c>
-      <c r="K20" s="89">
+      <c r="K20" s="74">
         <v>1</v>
       </c>
-      <c r="L20" s="89">
-        <v>0</v>
-      </c>
-      <c r="M20" s="89">
-        <v>0</v>
-      </c>
-      <c r="N20" s="89">
-        <v>0</v>
-      </c>
-      <c r="O20" s="89">
+      <c r="L20" s="74">
+        <v>0</v>
+      </c>
+      <c r="M20" s="74">
+        <v>0</v>
+      </c>
+      <c r="N20" s="74">
+        <v>0</v>
+      </c>
+      <c r="O20" s="74">
         <v>0</v>
       </c>
       <c r="R20">
@@ -2773,22 +2783,22 @@
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="J21" s="89">
+      <c r="J21" s="74">
         <v>100</v>
       </c>
-      <c r="K21" s="89">
+      <c r="K21" s="74">
         <v>1</v>
       </c>
-      <c r="L21" s="89">
-        <v>0</v>
-      </c>
-      <c r="M21" s="89">
-        <v>0</v>
-      </c>
-      <c r="N21" s="89">
-        <v>0</v>
-      </c>
-      <c r="O21" s="89">
+      <c r="L21" s="74">
+        <v>0</v>
+      </c>
+      <c r="M21" s="74">
+        <v>0</v>
+      </c>
+      <c r="N21" s="74">
+        <v>0</v>
+      </c>
+      <c r="O21" s="74">
         <v>0</v>
       </c>
       <c r="R21">
@@ -2812,12 +2822,12 @@
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="J22" s="89"/>
-      <c r="K22" s="89"/>
-      <c r="L22" s="89"/>
-      <c r="M22" s="89"/>
-      <c r="N22" s="89"/>
-      <c r="O22" s="89"/>
+      <c r="J22" s="74"/>
+      <c r="K22" s="74"/>
+      <c r="L22" s="74"/>
+      <c r="M22" s="74"/>
+      <c r="N22" s="74"/>
+      <c r="O22" s="74"/>
       <c r="R22">
         <v>100</v>
       </c>
@@ -2849,11 +2859,11 @@
         <f>SUM(S15:S22)</f>
         <v>1</v>
       </c>
-      <c r="T23" s="78">
+      <c r="T23" s="80">
         <f>SUM(T16:U20)</f>
         <v>7.9822552552706177E-2</v>
       </c>
-      <c r="U23" s="78"/>
+      <c r="U23" s="80"/>
       <c r="V23" s="6">
         <f>SUM(V16:V20)</f>
         <v>5.6035322666901982E-3</v>
@@ -2867,11 +2877,11 @@
       <c r="R24" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="T24" s="76">
+      <c r="T24" s="77">
         <f>T23/T11</f>
         <v>1.1188586983223026</v>
       </c>
-      <c r="U24" s="76"/>
+      <c r="U24" s="77"/>
       <c r="V24">
         <f>V23/V11</f>
         <v>1.1217922212073903</v>
@@ -2886,10 +2896,10 @@
       <c r="R25" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="T25" s="76">
+      <c r="T25" s="77">
         <v>1.3</v>
       </c>
-      <c r="U25" s="76"/>
+      <c r="U25" s="77"/>
       <c r="V25">
         <v>2.1</v>
       </c>
@@ -2902,11 +2912,11 @@
       <c r="R26" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="T26" s="81">
+      <c r="T26" s="78">
         <f>T11*T25</f>
         <v>9.274568671997388E-2</v>
       </c>
-      <c r="U26" s="81"/>
+      <c r="U26" s="78"/>
       <c r="V26" s="11">
         <f>V11*V25</f>
         <v>1.0489837188730092E-2</v>
@@ -2920,11 +2930,11 @@
       <c r="R27" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="T27" s="76">
+      <c r="T27" s="77">
         <f>T26/T23</f>
         <v>1.1618982825528494</v>
       </c>
-      <c r="U27" s="76"/>
+      <c r="U27" s="77"/>
       <c r="V27">
         <f>V26/V23</f>
         <v>1.8720044231896706</v>
@@ -2938,11 +2948,11 @@
       <c r="R28" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="T28" s="76">
+      <c r="T28" s="77">
         <f>(T24 -1) / (T25-1)</f>
         <v>0.39619566107434179</v>
       </c>
-      <c r="U28" s="76"/>
+      <c r="U28" s="77"/>
       <c r="V28">
         <f>(V24-1)/(V25-1)</f>
         <v>0.11072020109762754</v>
@@ -2962,22 +2972,22 @@
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="J30" s="77" t="s">
+      <c r="J30" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="K30" s="77"/>
-      <c r="L30" s="77"/>
-      <c r="M30" s="77"/>
-      <c r="N30" s="77"/>
-      <c r="O30" s="77"/>
-      <c r="P30" s="77"/>
-      <c r="S30" s="76" t="s">
+      <c r="K30" s="79"/>
+      <c r="L30" s="79"/>
+      <c r="M30" s="79"/>
+      <c r="N30" s="79"/>
+      <c r="O30" s="79"/>
+      <c r="P30" s="79"/>
+      <c r="S30" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="T30" s="76"/>
-      <c r="U30" s="76"/>
-      <c r="V30" s="76"/>
-      <c r="W30" s="76"/>
+      <c r="T30" s="77"/>
+      <c r="U30" s="77"/>
+      <c r="V30" s="77"/>
+      <c r="W30" s="77"/>
     </row>
     <row r="31" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="J31" s="9"/>
@@ -3376,11 +3386,11 @@
         <f>SUM(S33:S37)</f>
         <v>0.99460000000000004</v>
       </c>
-      <c r="T40" s="78">
+      <c r="T40" s="80">
         <f>SUM(T33:U37)</f>
         <v>9.274568671997388E-2</v>
       </c>
-      <c r="U40" s="78"/>
+      <c r="U40" s="80"/>
       <c r="V40" s="6">
         <f>SUM(V33:V37)</f>
         <v>1.0489837188730092E-2</v>
@@ -3394,11 +3404,11 @@
       <c r="R41" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="T41" s="79">
+      <c r="T41" s="81">
         <f>T40/T11</f>
         <v>1.3</v>
       </c>
-      <c r="U41" s="79"/>
+      <c r="U41" s="81"/>
       <c r="V41" s="12">
         <f>V40/V11</f>
         <v>2.1</v>
@@ -3413,10 +3423,10 @@
       <c r="R42" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="T42" s="74">
+      <c r="T42" s="82">
         <v>1.3</v>
       </c>
-      <c r="U42" s="74"/>
+      <c r="U42" s="82"/>
       <c r="V42" s="14">
         <v>2.1</v>
       </c>
@@ -3428,11 +3438,11 @@
       <c r="R43" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="T43" s="75" t="b">
+      <c r="T43" s="83" t="b">
         <f>T41=T42</f>
         <v>1</v>
       </c>
-      <c r="U43" s="76"/>
+      <c r="U43" s="77"/>
       <c r="V43" s="11" t="b">
         <f>V42=V41</f>
         <v>1</v>
@@ -3444,11 +3454,22 @@
     </row>
     <row r="44" spans="10:24" x14ac:dyDescent="0.35">
       <c r="R44" s="9"/>
-      <c r="T44" s="76"/>
-      <c r="U44" s="76"/>
+      <c r="T44" s="77"/>
+      <c r="U44" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="T43:U43"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="J30:P30"/>
+    <mergeCell ref="T28:U28"/>
+    <mergeCell ref="T27:U27"/>
+    <mergeCell ref="S30:W30"/>
+    <mergeCell ref="T40:U40"/>
+    <mergeCell ref="T41:U41"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="T24:U24"/>
     <mergeCell ref="T11:U11"/>
     <mergeCell ref="T25:U25"/>
     <mergeCell ref="T26:U26"/>
@@ -3456,17 +3477,6 @@
     <mergeCell ref="J1:P1"/>
     <mergeCell ref="S1:W1"/>
     <mergeCell ref="S13:W13"/>
-    <mergeCell ref="T27:U27"/>
-    <mergeCell ref="S30:W30"/>
-    <mergeCell ref="T40:U40"/>
-    <mergeCell ref="T41:U41"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="T24:U24"/>
-    <mergeCell ref="T42:U42"/>
-    <mergeCell ref="T43:U43"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="J30:P30"/>
-    <mergeCell ref="T28:U28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A13" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -3481,8 +3491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCBC5BEA-8F53-4533-8F93-063B86792D52}">
   <dimension ref="B1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3499,26 +3509,26 @@
       <c r="E1" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="86" t="s">
+      <c r="F1" s="88" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="83"/>
-      <c r="H1" s="82" t="s">
+      <c r="G1" s="85"/>
+      <c r="H1" s="84" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="83"/>
-      <c r="K1" s="86" t="s">
+      <c r="I1" s="85"/>
+      <c r="K1" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="L1" s="83"/>
-      <c r="M1" s="87" t="s">
+      <c r="L1" s="85"/>
+      <c r="M1" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="88"/>
-      <c r="O1" s="87" t="s">
+      <c r="N1" s="90"/>
+      <c r="O1" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="P1" s="88"/>
+      <c r="P1" s="90"/>
     </row>
     <row r="2" spans="2:16" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C2" s="15"/>
@@ -3610,7 +3620,7 @@
       <c r="C4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="84">
+      <c r="D4" s="86">
         <v>0.3</v>
       </c>
       <c r="E4" s="50">
@@ -3656,7 +3666,7 @@
       <c r="C5" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="85"/>
+      <c r="D5" s="87"/>
       <c r="E5" s="50">
         <v>3.6200000000000003E-2</v>
       </c>
@@ -4366,4 +4376,145 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{568F1B4E-D3F9-4C83-8878-D0FC1CFA8CEE}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="11.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="9"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="88" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="85"/>
+    </row>
+    <row r="2" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="9"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="91">
+        <v>0.92</v>
+      </c>
+      <c r="E3" s="43">
+        <v>0.88619999999999999</v>
+      </c>
+      <c r="F3" s="23">
+        <f>(E3-D3)/D3</f>
+        <v>-3.6739130434782663E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B4" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="86">
+        <v>0.3</v>
+      </c>
+      <c r="D4" s="91">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="E4" s="43">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="F4" s="23">
+        <f>(E4-D4)/D4</f>
+        <v>0.39473684210526316</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="87"/>
+      <c r="D5" s="91">
+        <v>3.3799999999999997E-2</v>
+      </c>
+      <c r="E5" s="43">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="F5" s="23">
+        <f>(E5-D5)/D5</f>
+        <v>0.30177514792899413</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B6" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="63">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="D6" s="91">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="E6" s="43">
+        <v>1.14E-2</v>
+      </c>
+      <c r="F6" s="23">
+        <f>(E6-D6)/D6</f>
+        <v>1.1923076923076925</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="64">
+        <v>0.53</v>
+      </c>
+      <c r="D7" s="92">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="E7" s="44">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="F7" s="24">
+        <f>(E7-D7)/D7</f>
+        <v>0.6875</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="C4:C5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Costs() function. This version of the codebase reflects manuscript version submitted to Lancet Planet Health.
</commit_message>
<xml_diff>
--- a/Data/Asthma/Healthcare use/CHARM Healthcare use probs by asthma control.xlsx
+++ b/Data/Asthma/Healthcare use/CHARM Healthcare use probs by asthma control.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smaya\Box\AA_Sigal_Documents\Climate - Health\Wildfire Asthma Microsim\Modeling\Data\Asthma\Healthcare use\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smaya\Box\AA_Sigal_Documents\IHPS\Climate - Health\Wildfire Asthma Microsim\Modeling\Data\Asthma\Healthcare use\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E584B02A-B74B-4911-B139-5F121B4A517A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF4F3FE-FDD5-4533-B9FC-6EE2E17B419D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24240" yWindow="-168" windowWidth="19176" windowHeight="10200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23112" yWindow="-564" windowWidth="19104" windowHeight="11196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Healthcare use by asthma contro" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="62">
   <si>
     <t>none</t>
   </si>
@@ -237,6 +237,24 @@
   </si>
   <si>
     <t>Mean proportions</t>
+  </si>
+  <si>
+    <t>FIRE - AFTER WITHIN STATE ADJUSTMENT (1 + 2 week fire effect)</t>
+  </si>
+  <si>
+    <t>FIRE - AFTER WITHIN STATE ADJUSTMENT (2 week fire effect, before recalibration)</t>
+  </si>
+  <si>
+    <t>FIRE - AFTER WITHIN STATE ADJUSTMENT (2 week fire effect, after recalibration)</t>
+  </si>
+  <si>
+    <t>no fire - any hru</t>
+  </si>
+  <si>
+    <t>adj factor</t>
+  </si>
+  <si>
+    <t>fire - any hru</t>
   </si>
 </sst>
 </file>
@@ -427,7 +445,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -631,6 +649,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="47">
     <border>
@@ -1252,7 +1276,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1286,9 +1310,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1298,13 +1319,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="18" xfId="44" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="18" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="19" xfId="44" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="19" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1313,44 +1331,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="12" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="12" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="13" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="13" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="26" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="26" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="28" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="28" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="30" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="30" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="33" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="33" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1362,10 +1377,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="36" xfId="44" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="36" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1374,7 +1389,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1383,7 +1398,7 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="40" xfId="44" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="40" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1395,21 +1410,9 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="18" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="40" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="36" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="19" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1423,56 +1426,62 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="16" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1494,11 +1503,15 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -1858,10 +1871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z44"/>
+  <dimension ref="A1:Z52"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="G31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M44" sqref="M44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1877,30 +1890,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="J1" s="79" t="s">
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="J1" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="S1" s="77" t="s">
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="S1" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="V1" s="77"/>
-      <c r="W1" s="77"/>
+      <c r="T1" s="73"/>
+      <c r="U1" s="73"/>
+      <c r="V1" s="73"/>
+      <c r="W1" s="73"/>
     </row>
     <row r="2" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B2" s="13" t="s">
@@ -2443,11 +2456,11 @@
         <f>SUM(S3:S10)</f>
         <v>1</v>
       </c>
-      <c r="T11" s="76">
+      <c r="T11" s="77">
         <f>SUM(T3:U10)</f>
         <v>7.1342835938441443E-2</v>
       </c>
-      <c r="U11" s="76"/>
+      <c r="U11" s="77"/>
       <c r="V11" s="6">
         <f>SUM(V3:V10)</f>
         <v>4.9951605660619484E-3</v>
@@ -2463,61 +2476,61 @@
       <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="J12" s="74"/>
-      <c r="K12" s="74"/>
-      <c r="L12" s="74"/>
-      <c r="M12" s="74"/>
-      <c r="N12" s="74"/>
-      <c r="O12" s="74"/>
+      <c r="J12" s="64"/>
+      <c r="K12" s="64"/>
+      <c r="L12" s="64"/>
+      <c r="M12" s="64"/>
+      <c r="N12" s="64"/>
+      <c r="O12" s="64"/>
       <c r="Y12" s="6"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J13" s="75" t="s">
+      <c r="J13" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="K13" s="74" t="s">
-        <v>0</v>
-      </c>
-      <c r="L13" s="74" t="s">
+      <c r="K13" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="L13" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="M13" s="74" t="s">
+      <c r="M13" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="N13" s="74" t="s">
+      <c r="N13" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="O13" s="74" t="s">
+      <c r="O13" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="S13" s="77" t="s">
+      <c r="S13" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="T13" s="77"/>
-      <c r="U13" s="77"/>
-      <c r="V13" s="77"/>
-      <c r="W13" s="77"/>
+      <c r="T13" s="73"/>
+      <c r="U13" s="73"/>
+      <c r="V13" s="73"/>
+      <c r="W13" s="73"/>
     </row>
     <row r="14" spans="1:26" ht="29" x14ac:dyDescent="0.35">
-      <c r="J14" s="74">
-        <v>0</v>
-      </c>
-      <c r="K14" s="74">
+      <c r="J14" s="64">
+        <v>0</v>
+      </c>
+      <c r="K14" s="64">
         <v>1</v>
       </c>
-      <c r="L14" s="74">
-        <v>0</v>
-      </c>
-      <c r="M14" s="74">
-        <v>0</v>
-      </c>
-      <c r="N14" s="74">
-        <v>0</v>
-      </c>
-      <c r="O14" s="74">
+      <c r="L14" s="64">
+        <v>0</v>
+      </c>
+      <c r="M14" s="64">
+        <v>0</v>
+      </c>
+      <c r="N14" s="64">
+        <v>0</v>
+      </c>
+      <c r="O14" s="64">
         <v>0</v>
       </c>
       <c r="S14" s="9" t="s">
@@ -2541,22 +2554,22 @@
       <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="74">
+      <c r="J15" s="64">
         <v>1</v>
       </c>
-      <c r="K15" s="74">
+      <c r="K15" s="64">
         <v>0.91410094600000003</v>
       </c>
-      <c r="L15" s="74">
+      <c r="L15" s="64">
         <v>3.9136651000000001E-2</v>
       </c>
-      <c r="M15" s="74">
+      <c r="M15" s="64">
         <v>4.0466157000000003E-2</v>
       </c>
-      <c r="N15" s="74">
+      <c r="N15" s="64">
         <v>4.3750170000000001E-3</v>
       </c>
-      <c r="O15" s="74">
+      <c r="O15" s="64">
         <v>1.921229E-3</v>
       </c>
       <c r="R15">
@@ -2564,241 +2577,241 @@
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="J16" s="74">
+      <c r="J16" s="64">
         <v>2</v>
       </c>
-      <c r="K16" s="74">
+      <c r="K16" s="64">
         <v>0.88382786199999996</v>
       </c>
-      <c r="L16" s="74">
+      <c r="L16" s="64">
         <v>4.9502009E-2</v>
       </c>
-      <c r="M16" s="74">
+      <c r="M16" s="64">
         <v>5.0963188999999999E-2</v>
       </c>
-      <c r="N16" s="74">
+      <c r="N16" s="64">
         <v>7.3192370000000001E-3</v>
       </c>
-      <c r="O16" s="74">
+      <c r="O16" s="64">
         <v>8.3877020000000004E-3</v>
       </c>
       <c r="R16">
         <v>1</v>
       </c>
       <c r="S16">
-        <v>5.4800000000000001E-2</v>
+        <v>6.3E-2</v>
       </c>
       <c r="T16" s="5">
         <f t="shared" ref="T16:W22" si="3">$S16*L4</f>
-        <v>1.0830467058556162E-3</v>
+        <v>1.2451084392135735E-3</v>
       </c>
       <c r="U16" s="5">
         <f t="shared" si="3"/>
-        <v>1.1202224958009766E-3</v>
+        <v>1.2878470298441885E-3</v>
       </c>
       <c r="V16" s="5">
         <f t="shared" si="3"/>
-        <v>1.2000686748422785E-4</v>
+        <v>1.3796409948004296E-4</v>
       </c>
       <c r="W16" s="5">
         <f t="shared" si="3"/>
-        <v>2.6339821650910135E-5</v>
+        <v>3.0281181824951431E-5</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>11</v>
       </c>
-      <c r="J17" s="74">
+      <c r="J17" s="64">
         <v>3</v>
       </c>
-      <c r="K17" s="74">
+      <c r="K17" s="64">
         <v>0.80730704200000003</v>
       </c>
-      <c r="L17" s="74">
+      <c r="L17" s="64">
         <v>8.0922303000000001E-2</v>
       </c>
-      <c r="M17" s="74">
+      <c r="M17" s="64">
         <v>7.6244352000000001E-2</v>
       </c>
-      <c r="N17" s="74">
+      <c r="N17" s="64">
         <v>1.7045363000000001E-2</v>
       </c>
-      <c r="O17" s="74">
+      <c r="O17" s="64">
         <v>1.8480940000000001E-2</v>
       </c>
       <c r="R17">
         <v>2</v>
       </c>
       <c r="S17">
-        <v>0.30780000000000002</v>
+        <v>0.36380000000000001</v>
       </c>
       <c r="T17" s="5">
         <f t="shared" si="3"/>
-        <v>6.6849164364182262E-3</v>
+        <v>7.901145547657409E-3</v>
       </c>
       <c r="U17" s="5">
         <f t="shared" si="3"/>
-        <v>6.9141398615959774E-3</v>
+        <v>8.1720730397940762E-3</v>
       </c>
       <c r="V17" s="5">
         <f t="shared" si="3"/>
-        <v>8.0868656895297087E-4</v>
+        <v>9.5581602919132813E-4</v>
       </c>
       <c r="W17" s="5">
         <f t="shared" si="3"/>
-        <v>5.1749717594333109E-4</v>
+        <v>6.1164870892847247E-4</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>12</v>
       </c>
-      <c r="J18" s="74">
+      <c r="J18" s="64">
         <v>4</v>
       </c>
-      <c r="K18" s="74">
+      <c r="K18" s="64">
         <v>0.61261256600000003</v>
       </c>
-      <c r="L18" s="74">
+      <c r="L18" s="64">
         <v>0.170907108</v>
       </c>
-      <c r="M18" s="74">
+      <c r="M18" s="64">
         <v>0.136274268</v>
       </c>
-      <c r="N18" s="74">
+      <c r="N18" s="64">
         <v>3.5211289E-2</v>
       </c>
-      <c r="O18" s="74">
+      <c r="O18" s="64">
         <v>4.4994768999999997E-2</v>
       </c>
       <c r="R18">
         <v>3</v>
       </c>
       <c r="S18">
-        <v>0.29799999999999999</v>
+        <v>0.27879999999999999</v>
       </c>
       <c r="T18" s="5">
         <f t="shared" si="3"/>
-        <v>1.0517290581837726E-2</v>
+        <v>9.8396664906589184E-3</v>
       </c>
       <c r="U18" s="5">
         <f t="shared" si="3"/>
-        <v>9.6868163118763988E-3</v>
+        <v>9.0626992877555039E-3</v>
       </c>
       <c r="V18" s="5">
         <f t="shared" si="3"/>
-        <v>1.7587204979237798E-3</v>
+        <v>1.6454069624870799E-3</v>
       </c>
       <c r="W18" s="5">
         <f t="shared" si="3"/>
-        <v>1.0011989606458303E-3</v>
+        <v>9.3669218197334723E-4</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="J19" s="74">
+      <c r="J19" s="64">
         <v>5</v>
       </c>
-      <c r="K19" s="74">
+      <c r="K19" s="64">
         <v>0.61261256600000003</v>
       </c>
-      <c r="L19" s="74">
+      <c r="L19" s="64">
         <v>0.170907108</v>
       </c>
-      <c r="M19" s="74">
+      <c r="M19" s="64">
         <v>0.136274268</v>
       </c>
-      <c r="N19" s="74">
+      <c r="N19" s="64">
         <v>3.5211289E-2</v>
       </c>
-      <c r="O19" s="74">
+      <c r="O19" s="64">
         <v>4.4994768999999997E-2</v>
       </c>
       <c r="R19">
         <v>4</v>
       </c>
       <c r="S19">
-        <v>0.25700000000000001</v>
+        <v>0.22239999999999999</v>
       </c>
       <c r="T19" s="5">
         <f t="shared" si="3"/>
-        <v>1.8773419727524568E-2</v>
+        <v>1.6245947655258611E-2</v>
       </c>
       <c r="U19" s="5">
         <f t="shared" si="3"/>
-        <v>1.4941379317222633E-2</v>
+        <v>1.2929816187355303E-2</v>
       </c>
       <c r="V19" s="5">
         <f t="shared" si="3"/>
-        <v>2.2438395551155972E-3</v>
+        <v>1.9417506500299952E-3</v>
       </c>
       <c r="W19" s="5">
         <f t="shared" si="3"/>
-        <v>1.662627463773969E-3</v>
+        <v>1.4387873460829988E-3</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>14</v>
       </c>
-      <c r="J20" s="74">
+      <c r="J20" s="64">
         <v>50</v>
       </c>
-      <c r="K20" s="74">
+      <c r="K20" s="64">
         <v>1</v>
       </c>
-      <c r="L20" s="74">
-        <v>0</v>
-      </c>
-      <c r="M20" s="74">
-        <v>0</v>
-      </c>
-      <c r="N20" s="74">
-        <v>0</v>
-      </c>
-      <c r="O20" s="74">
+      <c r="L20" s="64">
+        <v>0</v>
+      </c>
+      <c r="M20" s="64">
+        <v>0</v>
+      </c>
+      <c r="N20" s="64">
+        <v>0</v>
+      </c>
+      <c r="O20" s="64">
         <v>0</v>
       </c>
       <c r="R20">
         <v>5</v>
       </c>
       <c r="S20">
-        <v>7.6999999999999999E-2</v>
+        <v>7.0800000000000002E-2</v>
       </c>
       <c r="T20" s="5">
         <f t="shared" si="3"/>
-        <v>5.6247210856785667E-3</v>
+        <v>5.1718214657927603E-3</v>
       </c>
       <c r="U20" s="5">
         <f t="shared" si="3"/>
-        <v>4.476600028895497E-3</v>
+        <v>4.1161465200753398E-3</v>
       </c>
       <c r="V20" s="5">
         <f t="shared" si="3"/>
-        <v>6.7227877721362246E-4</v>
+        <v>6.181472393081101E-4</v>
       </c>
       <c r="W20" s="5">
         <f t="shared" si="3"/>
-        <v>4.9814130237585841E-4</v>
+        <v>4.5803122348325682E-4</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="J21" s="74">
+      <c r="J21" s="64">
         <v>100</v>
       </c>
-      <c r="K21" s="74">
+      <c r="K21" s="64">
         <v>1</v>
       </c>
-      <c r="L21" s="74">
-        <v>0</v>
-      </c>
-      <c r="M21" s="74">
-        <v>0</v>
-      </c>
-      <c r="N21" s="74">
-        <v>0</v>
-      </c>
-      <c r="O21" s="74">
+      <c r="L21" s="64">
+        <v>0</v>
+      </c>
+      <c r="M21" s="64">
+        <v>0</v>
+      </c>
+      <c r="N21" s="64">
+        <v>0</v>
+      </c>
+      <c r="O21" s="64">
         <v>0</v>
       </c>
       <c r="R21">
@@ -2822,12 +2835,12 @@
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="J22" s="74"/>
-      <c r="K22" s="74"/>
-      <c r="L22" s="74"/>
-      <c r="M22" s="74"/>
-      <c r="N22" s="74"/>
-      <c r="O22" s="74"/>
+      <c r="J22" s="64"/>
+      <c r="K22" s="64"/>
+      <c r="L22" s="64"/>
+      <c r="M22" s="64"/>
+      <c r="N22" s="64"/>
+      <c r="O22" s="64"/>
       <c r="R22">
         <v>100</v>
       </c>
@@ -2857,38 +2870,38 @@
       </c>
       <c r="S23" s="6">
         <f>SUM(S15:S22)</f>
-        <v>1</v>
-      </c>
-      <c r="T23" s="80">
+        <v>1.0042</v>
+      </c>
+      <c r="T23" s="75">
         <f>SUM(T16:U20)</f>
-        <v>7.9822552552706177E-2</v>
-      </c>
-      <c r="U23" s="80"/>
+        <v>7.5972271663405685E-2</v>
+      </c>
+      <c r="U23" s="75"/>
       <c r="V23" s="6">
         <f>SUM(V16:V20)</f>
-        <v>5.6035322666901982E-3</v>
+        <v>5.2990849804965563E-3</v>
       </c>
       <c r="W23" s="6">
         <f>SUM(W16:W20)</f>
-        <v>3.7058047243898988E-3</v>
+        <v>3.4754406422930271E-3</v>
       </c>
     </row>
     <row r="24" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="R24" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="T24" s="77">
+      <c r="T24" s="73">
         <f>T23/T11</f>
-        <v>1.1188586983223026</v>
-      </c>
-      <c r="U24" s="77"/>
+        <v>1.0648899873977364</v>
+      </c>
+      <c r="U24" s="73"/>
       <c r="V24">
         <f>V23/V11</f>
-        <v>1.1217922212073903</v>
+        <v>1.0608437727706947</v>
       </c>
       <c r="W24">
         <f>W23/W11</f>
-        <v>1.1514827998897459</v>
+        <v>1.0799031301621114</v>
       </c>
     </row>
     <row r="25" spans="1:23" ht="58" x14ac:dyDescent="0.35">
@@ -2896,10 +2909,10 @@
       <c r="R25" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="T25" s="77">
+      <c r="T25" s="73">
         <v>1.3</v>
       </c>
-      <c r="U25" s="77"/>
+      <c r="U25" s="73"/>
       <c r="V25">
         <v>2.1</v>
       </c>
@@ -2927,39 +2940,40 @@
       </c>
     </row>
     <row r="27" spans="1:23" ht="29" x14ac:dyDescent="0.35">
-      <c r="R27" s="9" t="s">
+      <c r="R27" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="T27" s="77">
+      <c r="S27" s="88"/>
+      <c r="T27" s="89">
         <f>T26/T23</f>
-        <v>1.1618982825528494</v>
-      </c>
-      <c r="U27" s="77"/>
-      <c r="V27">
+        <v>1.2207833817433105</v>
+      </c>
+      <c r="U27" s="89"/>
+      <c r="V27" s="88">
         <f>V26/V23</f>
-        <v>1.8720044231896706</v>
-      </c>
-      <c r="W27">
+        <v>1.9795563247878187</v>
+      </c>
+      <c r="W27" s="88">
         <f>W26/W23</f>
-        <v>1.3026681771917257</v>
+        <v>1.3890134754724022</v>
       </c>
     </row>
     <row r="28" spans="1:23" ht="58" x14ac:dyDescent="0.35">
       <c r="R28" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="T28" s="77">
+      <c r="T28" s="73">
         <f>(T24 -1) / (T25-1)</f>
-        <v>0.39619566107434179</v>
-      </c>
-      <c r="U28" s="77"/>
+        <v>0.21629995799245477</v>
+      </c>
+      <c r="U28" s="73"/>
       <c r="V28">
         <f>(V24-1)/(V25-1)</f>
-        <v>0.11072020109762754</v>
+        <v>5.5312520700631584E-2</v>
       </c>
       <c r="W28">
         <f>(W24-1)/(W25-1)</f>
-        <v>0.30296559977949178</v>
+        <v>0.15980626032422274</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="29" x14ac:dyDescent="0.35">
@@ -2968,26 +2982,26 @@
       </c>
       <c r="S29">
         <f>(5*T28 + V28+W28)/7</f>
-        <v>0.34209487232126118</v>
+        <v>0.18523122442673259</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="J30" s="79" t="s">
+      <c r="J30" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="K30" s="79"/>
-      <c r="L30" s="79"/>
-      <c r="M30" s="79"/>
-      <c r="N30" s="79"/>
-      <c r="O30" s="79"/>
-      <c r="P30" s="79"/>
-      <c r="S30" s="77" t="s">
+      <c r="K30" s="74"/>
+      <c r="L30" s="74"/>
+      <c r="M30" s="74"/>
+      <c r="N30" s="74"/>
+      <c r="O30" s="74"/>
+      <c r="P30" s="74"/>
+      <c r="S30" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="T30" s="77"/>
-      <c r="U30" s="77"/>
-      <c r="V30" s="77"/>
-      <c r="W30" s="77"/>
+      <c r="T30" s="73"/>
+      <c r="U30" s="73"/>
+      <c r="V30" s="73"/>
+      <c r="W30" s="73"/>
     </row>
     <row r="31" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="J31" s="9"/>
@@ -3062,49 +3076,50 @@
       </c>
       <c r="K33" s="3">
         <f>1-SUM(L33:O33)</f>
-        <v>0.9485594865765048</v>
+        <v>0.94591494256112685</v>
       </c>
       <c r="L33" s="3">
         <f>L4 *$T$27</f>
-        <v>2.296332312879857E-2</v>
+        <v>2.4127106207306053E-2</v>
       </c>
       <c r="M33" s="3">
         <f>M4 *$T$27</f>
-        <v>2.3751543685186519E-2</v>
+        <v>2.4955273845416927E-2</v>
       </c>
       <c r="N33" s="3">
         <f>N4 *$V$27</f>
-        <v>4.0995143566352407E-3</v>
+        <v>4.3350429479265852E-3</v>
       </c>
       <c r="O33" s="3">
         <f>O4 *$W$27</f>
-        <v>6.2613225287493166E-4</v>
+        <v>6.6763443822361154E-4</v>
       </c>
       <c r="P33" s="2">
         <f t="shared" ref="P33:P39" si="4">SUM(K33:O33)</f>
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="R33">
         <v>1</v>
       </c>
       <c r="S33">
-        <v>5.4800000000000001E-2</v>
+        <f>S16</f>
+        <v>6.3E-2</v>
       </c>
       <c r="T33" s="5">
         <f t="shared" ref="T33:W37" si="5">$S33*L33</f>
-        <v>1.2583901074581616E-3</v>
+        <v>1.5200076910602814E-3</v>
       </c>
       <c r="U33" s="5">
         <f t="shared" si="5"/>
-        <v>1.3015845939482213E-3</v>
+        <v>1.5721822522612664E-3</v>
       </c>
       <c r="V33" s="5">
         <f t="shared" si="5"/>
-        <v>2.2465338674361121E-4</v>
+        <v>2.7310770571937489E-4</v>
       </c>
       <c r="W33" s="5">
         <f t="shared" si="5"/>
-        <v>3.4312047457546254E-5</v>
+        <v>4.2060969608087526E-5</v>
       </c>
     </row>
     <row r="34" spans="10:24" x14ac:dyDescent="0.35">
@@ -3113,23 +3128,23 @@
       </c>
       <c r="K34" s="3">
         <f>1-SUM(L34:O34)</f>
-        <v>0.94155714069543794</v>
+        <v>0.93852776770872826</v>
       </c>
       <c r="L34" s="3">
         <f t="shared" ref="L34:M37" si="6">L5 *$T$27</f>
-        <v>2.5234544920349745E-2</v>
+        <v>2.6513433703450558E-2</v>
       </c>
       <c r="M34" s="3">
         <f t="shared" si="6"/>
-        <v>2.609982855918961E-2</v>
+        <v>2.7422569987281875E-2</v>
       </c>
       <c r="N34" s="3">
         <f>N5 *$V$27</f>
-        <v>4.9183392919234566E-3</v>
+        <v>5.2009116710260359E-3</v>
       </c>
       <c r="O34" s="3">
         <f>O5 *$W$27</f>
-        <v>2.1901465330993008E-3</v>
+        <v>2.3353169295133184E-3</v>
       </c>
       <c r="P34" s="2">
         <f t="shared" si="4"/>
@@ -3139,23 +3154,24 @@
         <v>2</v>
       </c>
       <c r="S34">
-        <v>0.30780000000000002</v>
+        <f t="shared" ref="S34:S37" si="7">S17</f>
+        <v>0.36380000000000001</v>
       </c>
       <c r="T34" s="5">
         <f t="shared" si="5"/>
-        <v>7.767192926483652E-3</v>
+        <v>9.6455871813153141E-3</v>
       </c>
       <c r="U34" s="5">
         <f t="shared" si="5"/>
-        <v>8.0335272305185629E-3</v>
+        <v>9.9763309613731463E-3</v>
       </c>
       <c r="V34" s="5">
         <f t="shared" si="5"/>
-        <v>1.51386483405404E-3</v>
+        <v>1.8920916659192718E-3</v>
       </c>
       <c r="W34" s="5">
         <f t="shared" si="5"/>
-        <v>6.7412710288796481E-4</v>
+        <v>8.4958829895694522E-4</v>
       </c>
     </row>
     <row r="35" spans="10:24" x14ac:dyDescent="0.35">
@@ -3164,49 +3180,50 @@
       </c>
       <c r="K35" s="3">
         <f>1-SUM(L35:O35)</f>
-        <v>0.90579973262866098</v>
+        <v>0.90088254002692392</v>
       </c>
       <c r="L35" s="3">
         <f t="shared" si="6"/>
-        <v>4.1006784779015142E-2</v>
+        <v>4.3085011957291704E-2</v>
       </c>
       <c r="M35" s="3">
         <f t="shared" si="6"/>
-        <v>3.7768775960315824E-2</v>
+        <v>3.9682900589056151E-2</v>
       </c>
       <c r="N35" s="3">
         <f>N6 *$V$27</f>
-        <v>1.1048095809623007E-2</v>
+        <v>1.1682839883218121E-2</v>
       </c>
       <c r="O35" s="3">
         <f>O6 *$W$27</f>
-        <v>4.3766108223850806E-3</v>
+        <v>4.6667075435101388E-3</v>
       </c>
       <c r="P35" s="2">
         <f t="shared" si="4"/>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="R35">
         <v>3</v>
       </c>
       <c r="S35">
-        <v>0.29799999999999999</v>
+        <f t="shared" si="7"/>
+        <v>0.27879999999999999</v>
       </c>
       <c r="T35" s="5">
         <f t="shared" si="5"/>
-        <v>1.2220021864146512E-2</v>
+        <v>1.2012101333692926E-2</v>
       </c>
       <c r="U35" s="5">
         <f t="shared" si="5"/>
-        <v>1.1255095236174115E-2</v>
+        <v>1.1063592684228855E-2</v>
       </c>
       <c r="V35" s="5">
         <f t="shared" si="5"/>
-        <v>3.2923325512676559E-3</v>
+        <v>3.2571757594412119E-3</v>
       </c>
       <c r="W35" s="5">
         <f t="shared" si="5"/>
-        <v>1.304230025070754E-3</v>
+        <v>1.3010780631306266E-3</v>
       </c>
     </row>
     <row r="36" spans="10:24" x14ac:dyDescent="0.35">
@@ -3215,49 +3232,50 @@
       </c>
       <c r="K36" s="3">
         <f>1-SUM(L36:O36)</f>
-        <v>0.82280351530586038</v>
+        <v>0.81358099172119325</v>
       </c>
       <c r="L36" s="3">
         <f t="shared" si="6"/>
-        <v>8.4874724276476951E-2</v>
+        <v>8.9176182186202407E-2</v>
       </c>
       <c r="M36" s="3">
         <f t="shared" si="6"/>
-        <v>6.7550050457788488E-2</v>
+        <v>7.0973492493340853E-2</v>
       </c>
       <c r="N36" s="3">
         <f>N7 *$V$27</f>
-        <v>1.6344270708577201E-2</v>
+        <v>1.7283294876023991E-2</v>
       </c>
       <c r="O36" s="3">
         <f>O7 *$W$27</f>
-        <v>8.4274392512970354E-3</v>
+        <v>8.9860387232394787E-3</v>
       </c>
       <c r="P36" s="2">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="R36">
         <v>4</v>
       </c>
       <c r="S36">
-        <v>0.25700000000000001</v>
+        <f t="shared" si="7"/>
+        <v>0.22239999999999999</v>
       </c>
       <c r="T36" s="5">
         <f t="shared" si="5"/>
-        <v>2.1812804139054578E-2</v>
+        <v>1.9832782918211413E-2</v>
       </c>
       <c r="U36" s="5">
         <f t="shared" si="5"/>
-        <v>1.7360362967651644E-2</v>
+        <v>1.5784504730519004E-2</v>
       </c>
       <c r="V36" s="5">
         <f t="shared" si="5"/>
-        <v>4.2004775721043407E-3</v>
+        <v>3.8438047804277352E-3</v>
       </c>
       <c r="W36" s="5">
         <f t="shared" si="5"/>
-        <v>2.1658518875833383E-3</v>
+        <v>1.9984950120484598E-3</v>
       </c>
     </row>
     <row r="37" spans="10:24" x14ac:dyDescent="0.35">
@@ -3266,49 +3284,50 @@
       </c>
       <c r="K37" s="3">
         <f>1-SUM(L37:O37)</f>
-        <v>0.82280351530586038</v>
+        <v>0.81358099172119325</v>
       </c>
       <c r="L37" s="3">
         <f t="shared" si="6"/>
-        <v>8.4874724276476951E-2</v>
+        <v>8.9176182186202407E-2</v>
       </c>
       <c r="M37" s="3">
         <f t="shared" si="6"/>
-        <v>6.7550050457788488E-2</v>
+        <v>7.0973492493340853E-2</v>
       </c>
       <c r="N37" s="3">
         <f>N8 *$V$27</f>
-        <v>1.6344270708577201E-2</v>
+        <v>1.7283294876023991E-2</v>
       </c>
       <c r="O37" s="3">
         <f>O8 *$W$27</f>
-        <v>8.4274392512970354E-3</v>
+        <v>8.9860387232394787E-3</v>
       </c>
       <c r="P37" s="2">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="R37">
         <v>5</v>
       </c>
       <c r="S37">
-        <v>7.6999999999999999E-2</v>
+        <f t="shared" si="7"/>
+        <v>7.0800000000000002E-2</v>
       </c>
       <c r="T37" s="5">
         <f t="shared" si="5"/>
-        <v>6.5353537692887254E-3</v>
+        <v>6.3136736987831309E-3</v>
       </c>
       <c r="U37" s="5">
         <f t="shared" si="5"/>
-        <v>5.2013538852497135E-3</v>
+        <v>5.0249232685285325E-3</v>
       </c>
       <c r="V37" s="5">
         <f t="shared" si="5"/>
-        <v>1.2585088445604446E-3</v>
+        <v>1.2236572772224986E-3</v>
       </c>
       <c r="W37" s="5">
         <f t="shared" si="5"/>
-        <v>6.4891282234987176E-4</v>
+        <v>6.362115416053551E-4</v>
       </c>
     </row>
     <row r="38" spans="10:24" x14ac:dyDescent="0.35">
@@ -3316,23 +3335,23 @@
         <v>50</v>
       </c>
       <c r="K38" s="3">
-        <f t="shared" ref="K38:O39" si="7">K9</f>
+        <f t="shared" ref="K38:O39" si="8">K9</f>
         <v>1</v>
       </c>
       <c r="L38" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M38" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="N38" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="N38:N39" si="9">N9 *$V$27</f>
         <v>0</v>
       </c>
       <c r="O38" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P38" s="2">
@@ -3348,23 +3367,23 @@
         <v>100</v>
       </c>
       <c r="K39" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="L39" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M39" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="N39" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O39" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P39" s="2">
@@ -3384,13 +3403,13 @@
       </c>
       <c r="S40" s="6">
         <f>SUM(S33:S37)</f>
-        <v>0.99460000000000004</v>
-      </c>
-      <c r="T40" s="80">
+        <v>0.99879999999999991</v>
+      </c>
+      <c r="T40" s="75">
         <f>SUM(T33:U37)</f>
-        <v>9.274568671997388E-2</v>
-      </c>
-      <c r="U40" s="80"/>
+        <v>9.2745686719973866E-2</v>
+      </c>
+      <c r="U40" s="75"/>
       <c r="V40" s="6">
         <f>SUM(V33:V37)</f>
         <v>1.0489837188730092E-2</v>
@@ -3401,14 +3420,23 @@
       </c>
     </row>
     <row r="41" spans="10:24" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="K41" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="L41" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="M41" t="s">
+        <v>60</v>
+      </c>
       <c r="R41" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="T41" s="81">
+      <c r="T41" s="76">
         <f>T40/T11</f>
-        <v>1.3</v>
-      </c>
-      <c r="U41" s="81"/>
+        <v>1.2999999999999998</v>
+      </c>
+      <c r="U41" s="76"/>
       <c r="V41" s="12">
         <f>V40/V11</f>
         <v>2.1</v>
@@ -3420,13 +3448,28 @@
       <c r="X41" s="12"/>
     </row>
     <row r="42" spans="10:24" ht="29" x14ac:dyDescent="0.35">
+      <c r="J42" s="14">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <f>1-K3</f>
+        <v>0</v>
+      </c>
+      <c r="L42" s="3">
+        <f>1-K32</f>
+        <v>0</v>
+      </c>
+      <c r="M42" t="e">
+        <f>L42/K42</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="R42" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="T42" s="82">
+      <c r="T42" s="71">
         <v>1.3</v>
       </c>
-      <c r="U42" s="82"/>
+      <c r="U42" s="71"/>
       <c r="V42" s="14">
         <v>2.1</v>
       </c>
@@ -3435,14 +3478,29 @@
       </c>
     </row>
     <row r="43" spans="10:24" x14ac:dyDescent="0.35">
+      <c r="J43" s="14">
+        <v>1</v>
+      </c>
+      <c r="K43">
+        <f t="shared" ref="K43:K49" si="10">1-K4</f>
+        <v>4.2876202386710416E-2</v>
+      </c>
+      <c r="L43" s="3">
+        <f t="shared" ref="L43:L49" si="11">1-K33</f>
+        <v>5.4085057438873152E-2</v>
+      </c>
+      <c r="M43">
+        <f t="shared" ref="M43:M49" si="12">L43/K43</f>
+        <v>1.2614236902575342</v>
+      </c>
       <c r="R43" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="T43" s="83" t="b">
+      <c r="T43" s="72" t="b">
         <f>T41=T42</f>
         <v>1</v>
       </c>
-      <c r="U43" s="77"/>
+      <c r="U43" s="73"/>
       <c r="V43" s="11" t="b">
         <f>V42=V41</f>
         <v>1</v>
@@ -3453,23 +3511,118 @@
       </c>
     </row>
     <row r="44" spans="10:24" x14ac:dyDescent="0.35">
+      <c r="J44" s="14">
+        <v>2</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="10"/>
+        <v>4.8490058618942511E-2</v>
+      </c>
+      <c r="L44" s="3">
+        <f t="shared" si="11"/>
+        <v>6.1472232291271744E-2</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="12"/>
+        <v>1.2677285621440306</v>
+      </c>
       <c r="R44" s="9"/>
-      <c r="T44" s="77"/>
-      <c r="U44" s="77"/>
+      <c r="T44" s="73"/>
+      <c r="U44" s="73"/>
+    </row>
+    <row r="45" spans="10:24" x14ac:dyDescent="0.35">
+      <c r="J45" s="14">
+        <v>3</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="10"/>
+        <v>7.7060491115046093E-2</v>
+      </c>
+      <c r="L45" s="3">
+        <f t="shared" si="11"/>
+        <v>9.9117459973076083E-2</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="12"/>
+        <v>1.2862292796071133</v>
+      </c>
+    </row>
+    <row r="46" spans="10:24" x14ac:dyDescent="0.35">
+      <c r="J46" s="14">
+        <v>4</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="10"/>
+        <v>0.14638624927485122</v>
+      </c>
+      <c r="L46" s="3">
+        <f t="shared" si="11"/>
+        <v>0.18641900827880675</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="12"/>
+        <v>1.2734734935983707</v>
+      </c>
+    </row>
+    <row r="47" spans="10:24" x14ac:dyDescent="0.35">
+      <c r="J47" s="14">
+        <v>5</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="10"/>
+        <v>0.14638624927485122</v>
+      </c>
+      <c r="L47" s="3">
+        <f t="shared" si="11"/>
+        <v>0.18641900827880675</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="12"/>
+        <v>1.2734734935983707</v>
+      </c>
+    </row>
+    <row r="48" spans="10:24" x14ac:dyDescent="0.35">
+      <c r="J48" s="14">
+        <v>50</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L48" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="M48" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="49" spans="10:13" x14ac:dyDescent="0.35">
+      <c r="J49" s="14">
+        <v>100</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L49" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="M49" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="52" spans="10:13" x14ac:dyDescent="0.35">
+      <c r="M52">
+        <f>AVERAGE(M43:M47)</f>
+        <v>1.272465703841084</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="T42:U42"/>
-    <mergeCell ref="T43:U43"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="J30:P30"/>
-    <mergeCell ref="T28:U28"/>
-    <mergeCell ref="T27:U27"/>
-    <mergeCell ref="S30:W30"/>
-    <mergeCell ref="T40:U40"/>
-    <mergeCell ref="T41:U41"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="T24:U24"/>
     <mergeCell ref="T11:U11"/>
     <mergeCell ref="T25:U25"/>
     <mergeCell ref="T26:U26"/>
@@ -3477,6 +3630,17 @@
     <mergeCell ref="J1:P1"/>
     <mergeCell ref="S1:W1"/>
     <mergeCell ref="S13:W13"/>
+    <mergeCell ref="T27:U27"/>
+    <mergeCell ref="S30:W30"/>
+    <mergeCell ref="T40:U40"/>
+    <mergeCell ref="T41:U41"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="T43:U43"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="J30:P30"/>
+    <mergeCell ref="T28:U28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A13" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -3489,883 +3653,1105 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCBC5BEA-8F53-4533-8F93-063B86792D52}">
-  <dimension ref="B1:Q22"/>
+  <dimension ref="B1:T22"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="13" max="13" width="0" style="22" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="0" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="0" style="21" hidden="1" customWidth="1"/>
     <col min="14" max="16" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" s="9" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:20" s="9" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C1" s="15"/>
       <c r="D1" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="88" t="s">
+      <c r="F1" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="85"/>
-      <c r="H1" s="84" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" s="85"/>
-      <c r="K1" s="88" t="s">
+      <c r="G1" s="80"/>
+      <c r="H1" s="79" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="80"/>
+      <c r="K1" s="83" t="s">
         <v>54</v>
       </c>
-      <c r="L1" s="85"/>
-      <c r="M1" s="89" t="s">
+      <c r="L1" s="80"/>
+      <c r="M1" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="90"/>
-      <c r="O1" s="89" t="s">
+      <c r="N1" s="85"/>
+      <c r="O1" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="P1" s="90"/>
-    </row>
-    <row r="2" spans="2:16" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="P1" s="85"/>
+      <c r="Q1" s="79" t="s">
+        <v>57</v>
+      </c>
+      <c r="R1" s="80"/>
+      <c r="S1" s="79" t="s">
+        <v>58</v>
+      </c>
+      <c r="T1" s="80"/>
+    </row>
+    <row r="2" spans="2:20" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C2" s="15"/>
       <c r="D2" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="39" t="s">
         <v>21</v>
       </c>
       <c r="G2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="15" t="s">
         <v>21</v>
       </c>
       <c r="I2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="42" t="s">
+      <c r="K2" s="39" t="s">
         <v>21</v>
       </c>
       <c r="L2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="42" t="s">
+      <c r="M2" s="39" t="s">
         <v>21</v>
       </c>
       <c r="N2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="42" t="s">
+      <c r="O2" s="39" t="s">
         <v>21</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="Q2" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="50">
-        <v>0.92300000000000004</v>
-      </c>
-      <c r="F3" s="55">
+      <c r="D3" s="20"/>
+      <c r="E3" s="47">
+        <v>0.92179999999999995</v>
+      </c>
+      <c r="F3" s="52">
         <v>0.91300000000000003</v>
       </c>
-      <c r="G3" s="56">
+      <c r="G3" s="22">
         <f>(F3-E3)/E3</f>
-        <v>-1.0834236186348871E-2</v>
-      </c>
-      <c r="H3" s="53">
+        <v>-9.5465393794748523E-3</v>
+      </c>
+      <c r="H3" s="50">
         <v>0.89219999999999999</v>
       </c>
-      <c r="I3" s="23">
+      <c r="I3" s="22">
         <f t="shared" ref="I3:I17" si="0">(H3-E3)/E3</f>
-        <v>-3.3369447453954551E-2</v>
-      </c>
-      <c r="K3" s="69">
+        <v>-3.2111087003688393E-2</v>
+      </c>
+      <c r="K3" s="59">
         <v>0.90900000000000003</v>
       </c>
-      <c r="L3" s="23">
+      <c r="L3" s="22">
         <f>(K3-E3)/E3</f>
-        <v>-1.516793066088842E-2</v>
-      </c>
-      <c r="M3" s="43">
+        <v>-1.3885875461054376E-2</v>
+      </c>
+      <c r="M3" s="40">
         <v>0.90580000000000005</v>
       </c>
-      <c r="N3" s="23">
+      <c r="N3" s="22">
         <f>(M3-E3)/E3</f>
-        <v>-1.8634886240520034E-2</v>
-      </c>
-      <c r="O3" s="43">
+        <v>-1.7357344326317969E-2</v>
+      </c>
+      <c r="O3" s="40">
         <v>0.91300000000000003</v>
       </c>
-      <c r="P3" s="23">
+      <c r="P3" s="22">
         <f>(O3-E3)/E3</f>
-        <v>-1.0834236186348871E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="C4" s="20" t="s">
+        <v>-9.5465393794748523E-3</v>
+      </c>
+      <c r="Q3" s="68">
+        <v>0.89090000000000003</v>
+      </c>
+      <c r="R3" s="22">
+        <f>(Q3-E3)/E3</f>
+        <v>-3.3521371230201699E-2</v>
+      </c>
+      <c r="S3" s="68">
+        <v>0.88639999999999997</v>
+      </c>
+      <c r="T3" s="22">
+        <f>(S3-E3)/E3</f>
+        <v>-3.8403124321978725E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="C4" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="86">
+      <c r="D4" s="81">
         <v>0.3</v>
       </c>
-      <c r="E4" s="50">
-        <v>3.2599999999999997E-2</v>
-      </c>
-      <c r="F4" s="55">
+      <c r="E4" s="47">
+        <v>3.8399999999999997E-2</v>
+      </c>
+      <c r="F4" s="52">
         <v>3.6400000000000002E-2</v>
       </c>
-      <c r="G4" s="56">
+      <c r="G4" s="22">
         <f t="shared" ref="G4:G12" si="1">(F4-E4)/E4</f>
-        <v>0.11656441717791427</v>
-      </c>
-      <c r="H4" s="53">
+        <v>-5.2083333333333204E-2</v>
+      </c>
+      <c r="H4" s="50">
         <v>4.5199999999999997E-2</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="22">
         <f t="shared" si="0"/>
-        <v>0.38650306748466262</v>
-      </c>
-      <c r="K4" s="69">
+        <v>0.17708333333333337</v>
+      </c>
+      <c r="K4" s="59">
         <v>3.9199999999999999E-2</v>
       </c>
-      <c r="L4" s="23">
+      <c r="L4" s="22">
         <f t="shared" ref="L4:L17" si="2">(K4-E4)/E4</f>
-        <v>0.20245398773006143</v>
-      </c>
-      <c r="M4" s="43">
+        <v>2.0833333333333391E-2</v>
+      </c>
+      <c r="M4" s="40">
         <v>4.1799999999999997E-2</v>
       </c>
-      <c r="N4" s="23">
+      <c r="N4" s="22">
         <f t="shared" ref="N4:N12" si="3">(M4-E4)/E4</f>
-        <v>0.28220858895705525</v>
-      </c>
-      <c r="O4" s="43">
+        <v>8.8541666666666685E-2</v>
+      </c>
+      <c r="O4" s="40">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="P4" s="23">
+      <c r="P4" s="22">
         <f t="shared" ref="P4:P17" si="4">(O4-E4)/E4</f>
-        <v>0.10429447852760738</v>
-      </c>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="C5" s="20" t="s">
+        <v>-6.2499999999999986E-2</v>
+      </c>
+      <c r="Q4" s="68">
+        <v>5.0799999999999998E-2</v>
+      </c>
+      <c r="R4" s="22">
+        <f t="shared" ref="R4:R6" si="5">(Q4-E4)/E4</f>
+        <v>0.32291666666666674</v>
+      </c>
+      <c r="S4" s="68">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="T4" s="22">
+        <f>(S4-E4)/E4</f>
+        <v>0.35416666666666674</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="C5" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="87"/>
-      <c r="E5" s="50">
-        <v>3.6200000000000003E-2</v>
-      </c>
-      <c r="F5" s="55">
+      <c r="D5" s="82"/>
+      <c r="E5" s="47">
+        <v>3.3700000000000001E-2</v>
+      </c>
+      <c r="F5" s="52">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="G5" s="56">
+      <c r="G5" s="22">
         <f t="shared" si="1"/>
-        <v>0.13259668508287289</v>
-      </c>
-      <c r="H5" s="53">
+        <v>0.21661721068249259</v>
+      </c>
+      <c r="H5" s="50">
         <v>4.6800000000000001E-2</v>
       </c>
-      <c r="I5" s="23">
+      <c r="I5" s="22">
         <f t="shared" si="0"/>
-        <v>0.29281767955801097</v>
-      </c>
-      <c r="K5" s="69">
+        <v>0.38872403560830859</v>
+      </c>
+      <c r="K5" s="59">
         <v>4.1599999999999998E-2</v>
       </c>
-      <c r="L5" s="23">
+      <c r="L5" s="22">
         <f t="shared" si="2"/>
-        <v>0.14917127071823189</v>
-      </c>
-      <c r="M5" s="43">
+        <v>0.23442136498516311</v>
+      </c>
+      <c r="M5" s="40">
         <v>4.24E-2</v>
       </c>
-      <c r="N5" s="23">
+      <c r="N5" s="22">
         <f t="shared" si="3"/>
-        <v>0.17127071823204409</v>
-      </c>
-      <c r="O5" s="43">
+        <v>0.25816023738872401</v>
+      </c>
+      <c r="O5" s="40">
         <v>4.1599999999999998E-2</v>
       </c>
-      <c r="P5" s="23">
+      <c r="P5" s="22">
         <f t="shared" si="4"/>
-        <v>0.14917127071823189</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="C6" s="20" t="s">
+        <v>0.23442136498516311</v>
+      </c>
+      <c r="Q5" s="68">
+        <v>4.24E-2</v>
+      </c>
+      <c r="R5" s="22">
+        <f t="shared" si="5"/>
+        <v>0.25816023738872401</v>
+      </c>
+      <c r="S5" s="68">
+        <v>4.2500000000000003E-2</v>
+      </c>
+      <c r="T5" s="22">
+        <f t="shared" ref="T5:T6" si="6">(S5-E5)/E5</f>
+        <v>0.26112759643916922</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="C6" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="63">
+      <c r="D6" s="56">
         <v>1.1200000000000001</v>
       </c>
-      <c r="E6" s="50">
-        <v>5.4000000000000003E-3</v>
-      </c>
-      <c r="F6" s="55">
+      <c r="E6" s="47">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="F6" s="52">
         <v>6.6E-3</v>
       </c>
-      <c r="G6" s="56">
+      <c r="G6" s="22">
         <f t="shared" si="1"/>
-        <v>0.22222222222222215</v>
-      </c>
-      <c r="H6" s="53">
+        <v>0.26923076923076927</v>
+      </c>
+      <c r="H6" s="50">
         <v>1.18E-2</v>
       </c>
-      <c r="I6" s="23">
+      <c r="I6" s="22">
         <f t="shared" si="0"/>
-        <v>1.1851851851851851</v>
-      </c>
-      <c r="K6" s="69">
+        <v>1.2692307692307694</v>
+      </c>
+      <c r="K6" s="59">
         <v>7.4000000000000003E-3</v>
       </c>
-      <c r="L6" s="23">
+      <c r="L6" s="22">
         <f t="shared" si="2"/>
-        <v>0.37037037037037035</v>
-      </c>
-      <c r="M6" s="43">
+        <v>0.42307692307692318</v>
+      </c>
+      <c r="M6" s="40">
         <v>6.4000000000000003E-3</v>
       </c>
-      <c r="N6" s="23">
+      <c r="N6" s="22">
         <f t="shared" si="3"/>
-        <v>0.18518518518518517</v>
-      </c>
-      <c r="O6" s="43">
+        <v>0.23076923076923089</v>
+      </c>
+      <c r="O6" s="40">
         <v>6.4000000000000003E-3</v>
       </c>
-      <c r="P6" s="23">
+      <c r="P6" s="22">
         <f t="shared" si="4"/>
-        <v>0.18518518518518517</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C7" s="20" t="s">
+        <v>0.23076923076923089</v>
+      </c>
+      <c r="Q6" s="68">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="R6" s="22">
+        <f t="shared" si="5"/>
+        <v>1.1153846153846154</v>
+      </c>
+      <c r="S6" s="68">
+        <v>1.12E-2</v>
+      </c>
+      <c r="T6" s="22">
+        <f t="shared" si="6"/>
+        <v>1.153846153846154</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C7" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="64">
+      <c r="D7" s="57">
         <v>0.53</v>
       </c>
-      <c r="E7" s="51">
+      <c r="E7" s="48">
         <v>3.2000000000000002E-3</v>
       </c>
-      <c r="F7" s="57">
+      <c r="F7" s="53">
         <v>3.3999999999999998E-3</v>
       </c>
-      <c r="G7" s="58">
+      <c r="G7" s="49">
         <f t="shared" si="1"/>
         <v>6.2499999999999889E-2</v>
       </c>
-      <c r="H7" s="54">
+      <c r="H7" s="51">
         <v>4.4000000000000003E-3</v>
       </c>
-      <c r="I7" s="52">
+      <c r="I7" s="49">
         <f t="shared" si="0"/>
         <v>0.375</v>
       </c>
-      <c r="K7" s="70">
+      <c r="K7" s="60">
         <v>3.2000000000000002E-3</v>
       </c>
-      <c r="L7" s="24">
+      <c r="L7" s="23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M7" s="44">
+      <c r="M7" s="41">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="N7" s="24">
+      <c r="N7" s="23">
         <f t="shared" si="3"/>
         <v>0.24999999999999997</v>
       </c>
-      <c r="O7" s="44">
+      <c r="O7" s="41">
         <v>3.3999999999999998E-3</v>
       </c>
-      <c r="P7" s="24">
+      <c r="P7" s="23">
         <f t="shared" si="4"/>
         <v>6.2499999999999889E-2</v>
       </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="Q7" s="69">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="R7" s="49">
+        <f>(Q7-E7)/E7</f>
+        <v>0.5625</v>
+      </c>
+      <c r="S7" s="69">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="T7" s="49">
+        <f>(S7-E7)/E7</f>
+        <v>0.62499999999999989</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="26">
+      <c r="D8" s="21"/>
+      <c r="E8" s="24">
         <v>0.91579999999999995</v>
       </c>
-      <c r="F8" s="66">
+      <c r="F8" s="33">
         <v>0.91149999999999998</v>
       </c>
-      <c r="G8" s="59">
+      <c r="G8" s="42">
         <f t="shared" si="1"/>
         <v>-4.6953483293295161E-3</v>
       </c>
-      <c r="H8" s="27">
+      <c r="H8" s="25">
         <v>0.88880000000000003</v>
       </c>
-      <c r="I8" s="28">
+      <c r="I8" s="26">
         <f t="shared" si="0"/>
         <v>-2.9482419742301719E-2</v>
       </c>
-      <c r="K8" s="71">
+      <c r="K8" s="61">
         <v>0.90380000000000005</v>
       </c>
-      <c r="L8" s="40">
+      <c r="L8" s="37">
         <f t="shared" si="2"/>
         <v>-1.3103297663245141E-2</v>
       </c>
-      <c r="M8" s="26">
+      <c r="M8" s="24">
         <v>0.90059999999999996</v>
       </c>
-      <c r="N8" s="45">
+      <c r="N8" s="42">
         <f t="shared" si="3"/>
         <v>-1.6597510373443976E-2</v>
       </c>
-      <c r="O8" s="46">
+      <c r="O8" s="43">
         <v>0.90780000000000005</v>
       </c>
-      <c r="P8" s="40">
+      <c r="P8" s="37">
         <f t="shared" si="4"/>
         <v>-8.7355317754967202E-3</v>
       </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="C9" s="20" t="s">
+      <c r="Q8" s="25"/>
+      <c r="R8" s="22">
+        <f>(Q8-E8)/E8</f>
+        <v>-1</v>
+      </c>
+      <c r="S8" s="25">
+        <v>0.89259999999999995</v>
+      </c>
+      <c r="T8" s="22">
+        <f>(S8-E8)/E8</f>
+        <v>-2.5333042148940818E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="C9" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="27">
         <v>4.1399999999999999E-2</v>
       </c>
-      <c r="F9" s="67">
+      <c r="F9" s="27">
         <v>4.2799999999999998E-2</v>
       </c>
-      <c r="G9" s="56">
+      <c r="G9" s="22">
         <f t="shared" si="1"/>
         <v>3.381642512077291E-2</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="21">
         <v>5.1200000000000002E-2</v>
       </c>
-      <c r="I9" s="30">
+      <c r="I9" s="28">
         <f t="shared" si="0"/>
         <v>0.23671497584541071</v>
       </c>
-      <c r="K9" s="72">
+      <c r="K9" s="62">
         <v>4.6399999999999997E-2</v>
       </c>
-      <c r="L9" s="39">
+      <c r="L9" s="36">
         <f t="shared" si="2"/>
         <v>0.12077294685990332</v>
       </c>
-      <c r="M9" s="47">
+      <c r="M9" s="44">
         <v>4.6800000000000001E-2</v>
       </c>
-      <c r="N9" s="23">
+      <c r="N9" s="22">
         <f t="shared" si="3"/>
         <v>0.1304347826086957</v>
       </c>
-      <c r="O9" s="38">
+      <c r="O9" s="35">
         <v>4.3799999999999999E-2</v>
       </c>
-      <c r="P9" s="39">
+      <c r="P9" s="36">
         <f t="shared" si="4"/>
         <v>5.797101449275361E-2</v>
       </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="C10" s="20" t="s">
+      <c r="Q9" s="21"/>
+      <c r="R9" s="22">
+        <f t="shared" ref="R9:R11" si="7">(Q9-E9)/E9</f>
+        <v>-1</v>
+      </c>
+      <c r="S9" s="21">
+        <v>4.5600000000000002E-2</v>
+      </c>
+      <c r="T9" s="22">
+        <f t="shared" ref="T9:T11" si="8">(S9-E9)/E9</f>
+        <v>0.1014492753623189</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="C10" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="27">
         <v>3.4599999999999999E-2</v>
       </c>
-      <c r="F10" s="67">
+      <c r="F10" s="27">
         <v>3.6400000000000002E-2</v>
       </c>
-      <c r="G10" s="56">
+      <c r="G10" s="22">
         <f t="shared" si="1"/>
         <v>5.2023121387283322E-2</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="21">
         <v>4.3799999999999999E-2</v>
       </c>
-      <c r="I10" s="30">
+      <c r="I10" s="28">
         <f t="shared" si="0"/>
         <v>0.26589595375722541</v>
       </c>
-      <c r="K10" s="72">
+      <c r="K10" s="62">
         <v>3.8800000000000001E-2</v>
       </c>
-      <c r="L10" s="39">
+      <c r="L10" s="36">
         <f t="shared" si="2"/>
         <v>0.1213872832369943</v>
       </c>
-      <c r="M10" s="47">
+      <c r="M10" s="44">
         <v>4.1399999999999999E-2</v>
       </c>
-      <c r="N10" s="23">
+      <c r="N10" s="22">
         <f t="shared" si="3"/>
         <v>0.19653179190751446</v>
       </c>
-      <c r="O10" s="38">
+      <c r="O10" s="35">
         <v>3.8800000000000001E-2</v>
       </c>
-      <c r="P10" s="39">
+      <c r="P10" s="36">
         <f t="shared" si="4"/>
         <v>0.1213872832369943</v>
       </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="C11" s="20" t="s">
+      <c r="Q10" s="21"/>
+      <c r="R10" s="22">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+      <c r="S10" s="21">
+        <v>4.6399999999999997E-2</v>
+      </c>
+      <c r="T10" s="22">
+        <f t="shared" si="8"/>
+        <v>0.34104046242774561</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="C11" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="27">
         <v>4.1999999999999997E-3</v>
       </c>
-      <c r="F11" s="67">
+      <c r="F11" s="27">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G11" s="56">
+      <c r="G11" s="22">
         <f t="shared" si="1"/>
         <v>0.19047619047619058</v>
       </c>
-      <c r="H11" s="25">
+      <c r="H11" s="21">
         <v>1.04E-2</v>
       </c>
-      <c r="I11" s="30">
+      <c r="I11" s="28">
         <f t="shared" si="0"/>
         <v>1.4761904761904763</v>
       </c>
-      <c r="K11" s="72">
+      <c r="K11" s="62">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="L11" s="39">
+      <c r="L11" s="36">
         <f t="shared" si="2"/>
         <v>0.42857142857142871</v>
       </c>
-      <c r="M11" s="47">
+      <c r="M11" s="44">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="N11" s="23">
+      <c r="N11" s="22">
         <f t="shared" si="3"/>
         <v>0.38095238095238093</v>
       </c>
-      <c r="O11" s="38">
+      <c r="O11" s="35">
         <v>4.7999999999999996E-3</v>
       </c>
-      <c r="P11" s="39">
+      <c r="P11" s="36">
         <f t="shared" si="4"/>
         <v>0.14285714285714282</v>
       </c>
-    </row>
-    <row r="12" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C12" s="20" t="s">
+      <c r="Q11" s="21"/>
+      <c r="R11" s="22">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+      <c r="S11" s="70">
+        <v>0.01</v>
+      </c>
+      <c r="T11" s="22">
+        <f t="shared" si="8"/>
+        <v>1.3809523809523812</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C12" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="31">
+      <c r="E12" s="29">
         <v>4.4000000000000003E-3</v>
       </c>
-      <c r="F12" s="68">
+      <c r="F12" s="29">
         <v>5.1999999999999998E-3</v>
       </c>
-      <c r="G12" s="60">
+      <c r="G12" s="23">
         <f t="shared" si="1"/>
         <v>0.18181818181818168</v>
       </c>
-      <c r="H12" s="32">
+      <c r="H12" s="30">
         <v>6.1999999999999998E-3</v>
       </c>
-      <c r="I12" s="33">
+      <c r="I12" s="31">
         <f t="shared" si="0"/>
         <v>0.40909090909090895</v>
       </c>
-      <c r="K12" s="73">
+      <c r="K12" s="63">
         <v>5.4000000000000003E-3</v>
       </c>
-      <c r="L12" s="41">
+      <c r="L12" s="38">
         <f t="shared" si="2"/>
         <v>0.22727272727272727</v>
       </c>
-      <c r="M12" s="48">
+      <c r="M12" s="45">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="N12" s="24">
+      <c r="N12" s="23">
         <f t="shared" si="3"/>
         <v>0.31818181818181801</v>
       </c>
-      <c r="O12" s="49">
+      <c r="O12" s="46">
         <v>5.1999999999999998E-3</v>
       </c>
-      <c r="P12" s="41">
+      <c r="P12" s="38">
         <f t="shared" si="4"/>
         <v>0.18181818181818168</v>
       </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="Q12" s="30"/>
+      <c r="R12" s="49">
+        <f>(Q12-E12)/E12</f>
+        <v>-1</v>
+      </c>
+      <c r="S12" s="30">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="T12" s="49">
+        <f>(S12-E12)/E12</f>
+        <v>0.22727272727272727</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="35">
+      <c r="E13" s="33">
         <v>0.91969999999999996</v>
       </c>
-      <c r="F13" s="61">
+      <c r="F13" s="54">
         <v>0.91149999999999998</v>
       </c>
-      <c r="G13" s="59">
+      <c r="G13" s="42">
         <f>(F13-E13)/E13</f>
         <v>-8.9159508535391809E-3</v>
       </c>
-      <c r="H13" s="36">
+      <c r="H13" s="25">
         <v>0.89090000000000003</v>
       </c>
-      <c r="I13" s="28">
+      <c r="I13" s="26">
         <f t="shared" si="0"/>
         <v>-3.1314559095357117E-2</v>
       </c>
-      <c r="K13" s="71">
+      <c r="K13" s="61">
         <v>0.90469999999999995</v>
       </c>
-      <c r="L13" s="40">
+      <c r="L13" s="37">
         <f t="shared" si="2"/>
         <v>-1.6309666195498548E-2</v>
       </c>
-      <c r="M13" s="26">
+      <c r="M13" s="24">
         <v>0.90190000000000003</v>
       </c>
-      <c r="N13" s="45">
+      <c r="N13" s="42">
         <f>(M13-E13)/E13</f>
         <v>-1.9354137218658179E-2</v>
       </c>
-      <c r="O13" s="46">
+      <c r="O13" s="43">
         <v>0.91390000000000005</v>
       </c>
-      <c r="P13" s="40">
+      <c r="P13" s="37">
         <f t="shared" si="4"/>
         <v>-6.3064042622593417E-3</v>
       </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="C14" s="20" t="s">
+      <c r="Q13" s="25"/>
+      <c r="R13" s="22">
+        <f>(Q13-E13)/E13</f>
+        <v>-1</v>
+      </c>
+      <c r="S13" s="25">
+        <v>0.88859999999999995</v>
+      </c>
+      <c r="T13" s="22">
+        <f>(S13-E13)/E13</f>
+        <v>-3.3815374578666978E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="C14" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="29">
+      <c r="E14" s="27">
         <v>3.9199999999999999E-2</v>
       </c>
-      <c r="F14" s="55">
+      <c r="F14" s="52">
         <v>4.2799999999999998E-2</v>
       </c>
-      <c r="G14" s="56">
+      <c r="G14" s="22">
         <f>(F14-E14)/E14</f>
         <v>9.1836734693877528E-2</v>
       </c>
-      <c r="H14" s="25">
+      <c r="H14" s="21">
         <v>5.0299999999999997E-2</v>
       </c>
-      <c r="I14" s="30">
+      <c r="I14" s="28">
         <f t="shared" si="0"/>
         <v>0.2831632653061224</v>
       </c>
-      <c r="K14" s="72">
+      <c r="K14" s="62">
         <v>4.9200000000000001E-2</v>
       </c>
-      <c r="L14" s="39">
+      <c r="L14" s="36">
         <f t="shared" si="2"/>
         <v>0.25510204081632659</v>
       </c>
-      <c r="M14" s="47">
+      <c r="M14" s="44">
         <v>4.9200000000000001E-2</v>
       </c>
-      <c r="N14" s="23">
+      <c r="N14" s="22">
         <f>(M14-E14)/E14</f>
         <v>0.25510204081632659</v>
       </c>
-      <c r="O14" s="38">
+      <c r="O14" s="35">
         <v>4.1599999999999998E-2</v>
       </c>
-      <c r="P14" s="39">
+      <c r="P14" s="36">
         <f t="shared" si="4"/>
         <v>6.1224489795918352E-2</v>
       </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="C15" s="20" t="s">
+      <c r="Q14" s="21"/>
+      <c r="R14" s="22">
+        <f t="shared" ref="R14:R16" si="9">(Q14-E14)/E14</f>
+        <v>-1</v>
+      </c>
+      <c r="S14" s="21">
+        <v>4.9399999999999999E-2</v>
+      </c>
+      <c r="T14" s="22">
+        <f t="shared" ref="T14:T16" si="10">(S14-E14)/E14</f>
+        <v>0.26020408163265307</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="C15" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E15" s="27">
         <v>3.2599999999999997E-2</v>
       </c>
-      <c r="F15" s="55">
+      <c r="F15" s="52">
         <v>3.6400000000000002E-2</v>
       </c>
-      <c r="G15" s="56">
+      <c r="G15" s="22">
         <f>(F15-E15)/E15</f>
         <v>0.11656441717791427</v>
       </c>
-      <c r="H15" s="25">
+      <c r="H15" s="21">
         <v>4.4200000000000003E-2</v>
       </c>
-      <c r="I15" s="30">
+      <c r="I15" s="28">
         <f t="shared" si="0"/>
         <v>0.35582822085889593</v>
       </c>
-      <c r="K15" s="72">
+      <c r="K15" s="62">
         <v>3.6799999999999999E-2</v>
       </c>
-      <c r="L15" s="39">
+      <c r="L15" s="36">
         <f t="shared" si="2"/>
         <v>0.12883435582822095</v>
       </c>
-      <c r="M15" s="47">
+      <c r="M15" s="44">
         <v>3.8600000000000002E-2</v>
       </c>
-      <c r="N15" s="23">
+      <c r="N15" s="22">
         <f>(M15-E15)/E15</f>
         <v>0.18404907975460141</v>
       </c>
-      <c r="O15" s="38">
+      <c r="O15" s="35">
         <v>3.5799999999999998E-2</v>
       </c>
-      <c r="P15" s="39">
+      <c r="P15" s="36">
         <f t="shared" si="4"/>
         <v>9.8159509202454046E-2</v>
       </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="C16" s="20" t="s">
+      <c r="Q15" s="21"/>
+      <c r="R15" s="22">
+        <f t="shared" si="9"/>
+        <v>-1</v>
+      </c>
+      <c r="S15" s="21">
+        <v>4.6600000000000003E-2</v>
+      </c>
+      <c r="T15" s="22">
+        <f t="shared" si="10"/>
+        <v>0.42944785276073638</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="C16" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="27">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="F16" s="55">
+      <c r="F16" s="52">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G16" s="56">
+      <c r="G16" s="22">
         <f>(F16-E16)/E16</f>
         <v>-0.10714285714285711</v>
       </c>
-      <c r="H16" s="25">
+      <c r="H16" s="21">
         <v>9.1999999999999998E-3</v>
       </c>
-      <c r="I16" s="30">
+      <c r="I16" s="28">
         <f t="shared" si="0"/>
         <v>0.64285714285714279</v>
       </c>
-      <c r="K16" s="72">
+      <c r="K16" s="62">
         <v>5.1999999999999998E-3</v>
       </c>
-      <c r="L16" s="39">
+      <c r="L16" s="36">
         <f t="shared" si="2"/>
         <v>-7.1428571428571466E-2</v>
       </c>
-      <c r="M16" s="47">
+      <c r="M16" s="44">
         <v>5.1999999999999998E-3</v>
       </c>
-      <c r="N16" s="23">
+      <c r="N16" s="22">
         <f>(M16-E16)/E16</f>
         <v>-7.1428571428571466E-2</v>
       </c>
-      <c r="O16" s="38">
+      <c r="O16" s="35">
         <v>4.7999999999999996E-3</v>
       </c>
-      <c r="P16" s="39">
+      <c r="P16" s="36">
         <f t="shared" si="4"/>
         <v>-0.14285714285714293</v>
       </c>
-    </row>
-    <row r="17" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C17" s="20" t="s">
+      <c r="Q16" s="21"/>
+      <c r="R16" s="22">
+        <f t="shared" si="9"/>
+        <v>-1</v>
+      </c>
+      <c r="S16" s="21">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="T16" s="22">
+        <f t="shared" si="10"/>
+        <v>0.92857142857142871</v>
+      </c>
+    </row>
+    <row r="17" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C17" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="31">
+      <c r="E17" s="29">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="F17" s="62">
+      <c r="F17" s="55">
         <v>5.1999999999999998E-3</v>
       </c>
-      <c r="G17" s="60">
+      <c r="G17" s="23">
         <f>(F17-E17)/E17</f>
         <v>0.44444444444444442</v>
       </c>
-      <c r="H17" s="32">
+      <c r="H17" s="30">
         <v>6.4000000000000003E-3</v>
       </c>
-      <c r="I17" s="33">
+      <c r="I17" s="31">
         <f t="shared" si="0"/>
         <v>0.7777777777777779</v>
       </c>
-      <c r="K17" s="73">
+      <c r="K17" s="63">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="L17" s="41">
+      <c r="L17" s="38">
         <f t="shared" si="2"/>
         <v>0.38888888888888895</v>
       </c>
-      <c r="M17" s="48">
+      <c r="M17" s="45">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="N17" s="24">
+      <c r="N17" s="23">
         <f>(M17-E17)/E17</f>
         <v>0.66666666666666674</v>
       </c>
-      <c r="O17" s="49">
+      <c r="O17" s="46">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="P17" s="41">
+      <c r="P17" s="38">
         <f t="shared" si="4"/>
         <v>0.38888888888888895</v>
       </c>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="Q17" s="30"/>
+      <c r="R17" s="49">
+        <f>(Q17-E17)/E17</f>
+        <v>-1</v>
+      </c>
+      <c r="S17" s="30">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="T17" s="49">
+        <f>(S17-E17)/E17</f>
+        <v>0.27777777777777779</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="C19" s="20" t="s">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="C19" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="37">
+      <c r="G19" s="34">
         <f>AVERAGE(G4,G9,G14)</f>
-        <v>8.07391923308549E-2</v>
-      </c>
-      <c r="I19" s="37">
+        <v>2.4523275493772412E-2</v>
+      </c>
+      <c r="I19" s="34">
         <f>AVERAGE(I4,I9,I14)</f>
-        <v>0.30212710287873196</v>
-      </c>
-      <c r="K19" s="20" t="s">
+        <v>0.23232052482828883</v>
+      </c>
+      <c r="K19" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="L19" s="65">
+      <c r="L19" s="58">
         <f>AVERAGE(L4,L9,L14)</f>
-        <v>0.19277632513543044</v>
-      </c>
-      <c r="N19" s="37">
+        <v>0.13223610700318777</v>
+      </c>
+      <c r="N19" s="34">
         <f>AVERAGE(N4,N9,N14)</f>
-        <v>0.22258180412735917</v>
-      </c>
-      <c r="P19" s="37">
+        <v>0.15802616336389633</v>
+      </c>
+      <c r="P19" s="34">
         <f>AVERAGE(P4,P9,P14)</f>
-        <v>7.4496660938759784E-2</v>
-      </c>
-      <c r="Q19">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="C20" s="20" t="s">
+        <v>1.8898501429557325E-2</v>
+      </c>
+      <c r="R19" s="34"/>
+      <c r="T19" s="34">
+        <f>AVERAGE(T4,T9,T14)</f>
+        <v>0.2386066745538796</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="C20" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="37">
+      <c r="G20" s="34">
         <f>AVERAGE(G5,G10,G15)</f>
-        <v>0.1003947412160235</v>
-      </c>
-      <c r="I20" s="37">
+        <v>0.12840158308256339</v>
+      </c>
+      <c r="I20" s="34">
         <f>AVERAGE(I5,I10,I15)</f>
-        <v>0.30484728472471079</v>
-      </c>
-      <c r="K20" s="20" t="s">
+        <v>0.33681607007480996</v>
+      </c>
+      <c r="K20" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="L20" s="65">
-        <f t="shared" ref="L20:N21" si="5">AVERAGE(L5,L10,L15)</f>
-        <v>0.13313096992781573</v>
-      </c>
-      <c r="N20" s="37">
-        <f t="shared" si="5"/>
-        <v>0.18395052996471997</v>
-      </c>
-      <c r="P20" s="37">
+      <c r="L20" s="58">
+        <f t="shared" ref="L20:N21" si="11">AVERAGE(L5,L10,L15)</f>
+        <v>0.16154766801679279</v>
+      </c>
+      <c r="N20" s="34">
+        <f t="shared" si="11"/>
+        <v>0.21291370301694665</v>
+      </c>
+      <c r="P20" s="34">
         <f>AVERAGE(P5,P10,P15)</f>
-        <v>0.12290602105256009</v>
-      </c>
-      <c r="Q20">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="C21" s="20" t="s">
+        <v>0.15132271914153714</v>
+      </c>
+      <c r="R20" s="34"/>
+      <c r="T20" s="34">
+        <f>AVERAGE(T5,T10,T15)</f>
+        <v>0.34387197054255036</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="C21" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="G21" s="37">
+      <c r="G21" s="34">
         <f>AVERAGE(G6,G11,G16)</f>
-        <v>0.10185185185185187</v>
-      </c>
-      <c r="I21" s="37">
+        <v>0.11752136752136759</v>
+      </c>
+      <c r="I21" s="34">
         <f>AVERAGE(I6,I11,I16)</f>
-        <v>1.101410934744268</v>
-      </c>
-      <c r="K21" s="20" t="s">
+        <v>1.1294261294261294</v>
+      </c>
+      <c r="K21" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="L21" s="65">
-        <f t="shared" si="5"/>
-        <v>0.24250440917107585</v>
-      </c>
-      <c r="N21" s="37">
-        <f t="shared" si="5"/>
-        <v>0.16490299823633153</v>
-      </c>
-      <c r="P21" s="37">
+      <c r="L21" s="58">
+        <f t="shared" si="11"/>
+        <v>0.26007326007326015</v>
+      </c>
+      <c r="N21" s="34">
+        <f t="shared" si="11"/>
+        <v>0.1800976800976801</v>
+      </c>
+      <c r="P21" s="34">
         <f>AVERAGE(P6,P11,P16)</f>
-        <v>6.1728395061728364E-2</v>
-      </c>
-      <c r="Q21">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="C22" s="20" t="s">
+        <v>7.6923076923076941E-2</v>
+      </c>
+      <c r="R21" s="34"/>
+      <c r="T21" s="34">
+        <f>AVERAGE(T6,T11,T16)</f>
+        <v>1.1544566544566546</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="C22" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="37">
+      <c r="G22" s="34">
         <f>AVERAGE(G7,G12,G17)</f>
         <v>0.22958754208754198</v>
       </c>
-      <c r="I22" s="37">
+      <c r="I22" s="34">
         <f>AVERAGE(I7,I12,I17)</f>
         <v>0.52062289562289565</v>
       </c>
-      <c r="K22" s="20" t="s">
+      <c r="K22" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="L22" s="65">
+      <c r="L22" s="58">
         <f>AVERAGE(L7,L12,L17)</f>
         <v>0.20538720538720542</v>
       </c>
-      <c r="N22" s="37">
+      <c r="N22" s="34">
         <f>AVERAGE(N7,N12,N17)</f>
         <v>0.4116161616161616</v>
       </c>
-      <c r="P22" s="37">
+      <c r="P22" s="34">
         <f>AVERAGE(P7,P12,P17)</f>
         <v>0.21106902356902349</v>
       </c>
-      <c r="Q22">
-        <v>39</v>
+      <c r="R22" s="34"/>
+      <c r="T22" s="34">
+        <f>AVERAGE(T7,T12,T17)</f>
+        <v>0.37668350168350168</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="K1:L1"/>
@@ -4380,18 +4766,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{568F1B4E-D3F9-4C83-8878-D0FC1CFA8CEE}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="11.08984375" customWidth="1"/>
     <col min="4" max="4" width="11.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="9"/>
       <c r="B1" s="15"/>
       <c r="C1" s="16" t="s">
@@ -4400,12 +4787,12 @@
       <c r="D1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="88" t="s">
+      <c r="E1" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="85"/>
-    </row>
-    <row r="2" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="F1" s="80"/>
+    </row>
+    <row r="2" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="9"/>
       <c r="B2" s="15"/>
       <c r="C2" s="17" t="s">
@@ -4414,106 +4801,112 @@
       <c r="D2" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="42" t="s">
+      <c r="E2" s="39" t="s">
         <v>21</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="91">
-        <v>0.92</v>
-      </c>
-      <c r="E3" s="43">
-        <v>0.88619999999999999</v>
-      </c>
-      <c r="F3" s="23">
+      <c r="C3" s="20"/>
+      <c r="D3" s="66">
+        <v>0.92179999999999995</v>
+      </c>
+      <c r="E3" s="59">
+        <v>0.88639999999999997</v>
+      </c>
+      <c r="F3" s="22">
         <f>(E3-D3)/D3</f>
-        <v>-3.6739130434782663E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="20" t="s">
+        <v>-3.8403124321978725E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B4" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="86">
+      <c r="C4" s="81">
         <v>0.3</v>
       </c>
-      <c r="D4" s="91">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="E4" s="43">
-        <v>5.2999999999999999E-2</v>
-      </c>
-      <c r="F4" s="23">
+      <c r="D4" s="66">
+        <v>3.8399999999999997E-2</v>
+      </c>
+      <c r="E4" s="59">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="F4" s="22">
         <f>(E4-D4)/D4</f>
-        <v>0.39473684210526316</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="20" t="s">
+        <v>0.35416666666666674</v>
+      </c>
+      <c r="G4" s="86">
+        <f>(F4*E4 + F5*E5) / (E4+E5)</f>
+        <v>0.31232369857493503</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B5" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="87"/>
-      <c r="D5" s="91">
-        <v>3.3799999999999997E-2</v>
-      </c>
-      <c r="E5" s="43">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="F5" s="23">
+      <c r="C5" s="82"/>
+      <c r="D5" s="66">
+        <v>3.3700000000000001E-2</v>
+      </c>
+      <c r="E5" s="59">
+        <v>4.2500000000000003E-2</v>
+      </c>
+      <c r="F5" s="22">
         <f>(E5-D5)/D5</f>
-        <v>0.30177514792899413</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="20" t="s">
+        <v>0.26112759643916922</v>
+      </c>
+      <c r="G5" s="86"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B6" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="63">
+      <c r="C6" s="56">
         <v>1.1200000000000001</v>
       </c>
-      <c r="D6" s="91">
+      <c r="D6" s="66">
         <v>5.1999999999999998E-3</v>
       </c>
-      <c r="E6" s="43">
-        <v>1.14E-2</v>
-      </c>
-      <c r="F6" s="23">
+      <c r="E6" s="59">
+        <v>1.12E-2</v>
+      </c>
+      <c r="F6" s="22">
         <f>(E6-D6)/D6</f>
-        <v>1.1923076923076925</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="20" t="s">
+        <v>1.153846153846154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="64">
+      <c r="C7" s="57">
         <v>0.53</v>
       </c>
-      <c r="D7" s="92">
+      <c r="D7" s="67">
         <v>3.2000000000000002E-3</v>
       </c>
-      <c r="E7" s="44">
-        <v>5.4000000000000003E-3</v>
-      </c>
-      <c r="F7" s="24">
+      <c r="E7" s="60">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="F7" s="23">
         <f>(E7-D7)/D7</f>
-        <v>0.6875</v>
+        <v>0.62499999999999989</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="C4:C5"/>
+    <mergeCell ref="G4:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>